<commit_message>
Add secondary other purpose for 2011 EC definition
- restore other purpose and instead add another purpose for EC 2011
  nanomaterial defintion
- add technique hashes
- bump dependency versions
- bump NanoDefiner e-tool version to 2.0.0
- update changelog
</commit_message>
<xml_diff>
--- a/config/knowledge/production/V1.0.2/xlsx/measurement_technique_performance_dict_V1.0.2.xlsx
+++ b/config/knowledge/production/V1.0.2/xlsx/measurement_technique_performance_dict_V1.0.2.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -474,7 +474,7 @@
 food_regulation = Food regulation
 biocide_regulation = Biocide regulation
 other = Other (e.g. informative, scientific)
-other_2011 = Other (e.g. informative, scientific), NanoDefine approach aligned with EC 2011 nanomaterial definition</t>
+other_2011 = Other (e.g. informative, scientific), NanoDefine approach oriented towards the EC 2011 nanomaterial definition</t>
   </si>
   <si>
     <t xml:space="preserve">Purpose support</t>
@@ -1162,6 +1162,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1221,12 +1222,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1250,1654 +1255,1654 @@
   <dimension ref="A1:K86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="144.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="227.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="52.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="56.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="51.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="144.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="227.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="52.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="56.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="51.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="K7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="0" t="s">
+      <c r="K8" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K9" s="0" t="s">
+      <c r="K9" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="K10" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="K13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="K17" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="K18" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="0" t="s">
+      <c r="K19" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="K20" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" customFormat="false" ht="169.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" s="1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="J34" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="J39" s="0" t="s">
+      <c r="J39" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" s="1" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="J41" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="H42" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J42" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="H44" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="J44" s="1" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J45" s="0" t="s">
+      <c r="J45" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K46" s="0" t="s">
+      <c r="K46" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="J47" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="H48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J48" s="0" t="s">
+      <c r="J48" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J49" s="0" t="s">
+      <c r="J49" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="H50" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J50" s="0" t="s">
+      <c r="J50" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="J51" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="H52" s="0" t="s">
+      <c r="H52" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="J52" s="0" t="s">
+      <c r="J52" s="1" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J53" s="0" t="s">
+      <c r="J53" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="J54" s="0" t="s">
+      <c r="J54" s="1" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="J55" s="0" t="s">
+      <c r="J55" s="1" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J56" s="0" t="s">
+      <c r="J56" s="1" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J57" s="0" t="s">
+      <c r="J57" s="1" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J58" s="0" t="s">
+      <c r="J58" s="1" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="J59" s="0" t="s">
+      <c r="J59" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="J61" s="0" t="s">
+      <c r="J61" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J62" s="0" t="s">
+      <c r="J62" s="1" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="J63" s="0" t="s">
+      <c r="J63" s="1" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="J64" s="0" t="s">
+      <c r="J64" s="1" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J65" s="0" t="s">
+      <c r="J65" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="J66" s="0" t="s">
+      <c r="J66" s="1" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="J67" s="0" t="s">
+      <c r="J67" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="J68" s="0" t="s">
+      <c r="J68" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="J69" s="0" t="s">
+      <c r="J69" s="1" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="J70" s="0" t="s">
+      <c r="J70" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J71" s="0" t="s">
+      <c r="J71" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="J72" s="0" t="s">
+      <c r="J72" s="1" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="J73" s="0" t="s">
+      <c r="J73" s="1" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="J74" s="0" t="s">
+      <c r="J74" s="1" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="J75" s="0" t="s">
+      <c r="J75" s="1" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="J76" s="0" t="s">
+      <c r="J76" s="1" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="J77" s="0" t="s">
+      <c r="J77" s="1" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="J78" s="0" t="s">
+      <c r="J78" s="1" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="J79" s="0" t="s">
+      <c r="J79" s="1" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="J80" s="0" t="s">
+      <c r="J80" s="1" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J81" s="0" t="s">
+      <c r="J81" s="1" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="E82" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="J82" s="0" t="s">
+      <c r="J82" s="1" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="E83" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="J83" s="0" t="s">
+      <c r="J83" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="J84" s="0" t="s">
+      <c r="J84" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="J85" s="0" t="s">
+      <c r="J85" s="1" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="J86" s="0" t="s">
+      <c r="J86" s="1" t="s">
         <v>329</v>
       </c>
     </row>

</xml_diff>